<commit_message>
i finished the list page all thats left is the remove item
</commit_message>
<xml_diff>
--- a/Gannt chart.xlsx
+++ b/Gannt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f95c939b2a42fc3/Desktop/school/Curent Quarter/CSC-132 Scienc of computing 3/132-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{0162FB3D-09DC-4E15-8FE8-546A3869AE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C6FC7A32-EC89-45CA-AA0B-242B76123D99}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{0162FB3D-09DC-4E15-8FE8-546A3869AE03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AE8340FB-7E64-4B15-B229-E0EA9C81A9AC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75535606-2F23-4DAC-A04B-A59C6231BC07}"/>
   </bookViews>
@@ -396,10 +396,10 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3</c:v>
@@ -511,7 +511,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1466,13 +1466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CD71C8-C6B1-4450-AAF1-4F87C58550E0}">
   <dimension ref="B4:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1558,11 +1559,11 @@
         <v>43934</v>
       </c>
       <c r="D10" s="5">
-        <v>43949</v>
+        <v>43968</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1573,11 +1574,11 @@
         <v>43943</v>
       </c>
       <c r="D11" s="5">
-        <v>43949</v>
+        <v>43968</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>